<commit_message>
Revert "Merge branch 'main' into Anim2"
This reverts commit c68725a98d0c007463fda03e8a4b961253ff42b6, reversing
changes made to 979087735ae22af35b07b7e509140d6b4c76d503.
</commit_message>
<xml_diff>
--- a/MakeAGame/LubanTool/GameConfig/Datas/Relic.xlsx
+++ b/MakeAGame/LubanTool/GameConfig/Datas/Relic.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
   <si>
     <t>##var</t>
   </si>
@@ -206,72 +206,6 @@
   </si>
   <si>
     <t>Relic6</t>
-  </si>
-  <si>
-    <t>鱼鳞</t>
-  </si>
-  <si>
-    <t>这些鳞片是剥自可怕的巨型海怪。它们可以让你在水中呼吸，并进行长时间的潜水。但取得它们的代价是任何人都无法想象的。</t>
-  </si>
-  <si>
-    <t>每当你造成小于等于{0}点且非Miss伤害时，将伤害提升为{0}</t>
-  </si>
-  <si>
-    <t>Relic7</t>
-  </si>
-  <si>
-    <t>伤害值</t>
-  </si>
-  <si>
-    <t>废品回收机</t>
-  </si>
-  <si>
-    <t>这个破烂回收机可以将无用的垃圾和装置重新变成有用的东西。但使用它需要小心谨慎，因为有时候回收的东西可能远比你想象的更加危险。</t>
-  </si>
-  <si>
-    <t>每使用{0}张死面牌，随机获得一张普通品质的学者牌</t>
-  </si>
-  <si>
-    <t>Relic8</t>
-  </si>
-  <si>
-    <t>使用死面数</t>
-  </si>
-  <si>
-    <t>水晶球</t>
-  </si>
-  <si>
-    <t>这些法珠和水晶球是由神秘巫师制成的。它们能够让你看到未来和未知，但数据可能会来得非常模糊和不可靠。</t>
-  </si>
-  <si>
-    <t>在每场战斗的前{0}秒混沌值损耗减少{1}%</t>
-  </si>
-  <si>
-    <t>Relic9</t>
-  </si>
-  <si>
-    <t>10,10</t>
-  </si>
-  <si>
-    <t>秒数，减少比例</t>
-  </si>
-  <si>
-    <t>符纸</t>
-  </si>
-  <si>
-    <t>些护身符能够保护你不受死气的侵害。当你使用它们时，你会感到一股强烈的保护力量。</t>
-  </si>
-  <si>
-    <t>抵消下{0}次生面牌受到的超过{1}点伤害的攻击</t>
-  </si>
-  <si>
-    <t>Relic10</t>
-  </si>
-  <si>
-    <t>5,10</t>
-  </si>
-  <si>
-    <t>抵消次数，伤害值</t>
   </si>
 </sst>
 </file>
@@ -322,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -443,21 +377,6 @@
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
@@ -471,7 +390,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -544,19 +463,16 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2120,7 +2036,7 @@
       <c r="E9" t="s" s="21">
         <v>62</v>
       </c>
-      <c r="F9" t="s" s="24">
+      <c r="F9" t="s" s="15">
         <v>63</v>
       </c>
       <c r="G9" t="s" s="15">
@@ -2156,33 +2072,17 @@
     </row>
     <row r="10" ht="16" customHeight="1">
       <c r="A10" s="19"/>
-      <c r="B10" s="20">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s" s="21">
-        <v>65</v>
-      </c>
-      <c r="D10" t="s" s="21">
-        <v>66</v>
-      </c>
-      <c r="E10" t="s" s="21">
-        <v>67</v>
-      </c>
-      <c r="F10" t="s" s="24">
-        <v>63</v>
-      </c>
-      <c r="G10" t="s" s="21">
-        <v>68</v>
-      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
-      <c r="K10" t="s" s="21">
-        <v>35</v>
-      </c>
-      <c r="L10" t="s" s="21">
-        <v>69</v>
-      </c>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
       <c r="M10" s="19"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -2208,33 +2108,17 @@
     </row>
     <row r="11" ht="16" customHeight="1">
       <c r="A11" s="19"/>
-      <c r="B11" s="20">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s" s="21">
-        <v>70</v>
-      </c>
-      <c r="D11" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="E11" t="s" s="21">
-        <v>72</v>
-      </c>
-      <c r="F11" t="s" s="24">
-        <v>63</v>
-      </c>
-      <c r="G11" t="s" s="21">
-        <v>73</v>
-      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
-      <c r="K11" t="s" s="21">
-        <v>35</v>
-      </c>
-      <c r="L11" t="s" s="21">
-        <v>74</v>
-      </c>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
       <c r="M11" s="19"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -2260,33 +2144,17 @@
     </row>
     <row r="12" ht="16" customHeight="1">
       <c r="A12" s="19"/>
-      <c r="B12" s="20">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s" s="21">
-        <v>75</v>
-      </c>
-      <c r="D12" t="s" s="21">
-        <v>76</v>
-      </c>
-      <c r="E12" t="s" s="21">
-        <v>77</v>
-      </c>
-      <c r="F12" t="s" s="24">
-        <v>63</v>
-      </c>
-      <c r="G12" t="s" s="21">
-        <v>78</v>
-      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
-      <c r="K12" t="s" s="21">
-        <v>79</v>
-      </c>
-      <c r="L12" t="s" s="21">
-        <v>80</v>
-      </c>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
       <c r="M12" s="19"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
@@ -2312,33 +2180,17 @@
     </row>
     <row r="13" ht="16" customHeight="1">
       <c r="A13" s="19"/>
-      <c r="B13" s="20">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s" s="21">
-        <v>81</v>
-      </c>
-      <c r="D13" t="s" s="21">
-        <v>82</v>
-      </c>
-      <c r="E13" t="s" s="21">
-        <v>83</v>
-      </c>
-      <c r="F13" t="s" s="15">
-        <v>63</v>
-      </c>
-      <c r="G13" t="s" s="21">
-        <v>84</v>
-      </c>
-      <c r="H13" s="25"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="24"/>
       <c r="I13" s="19"/>
       <c r="J13" s="21"/>
-      <c r="K13" t="s" s="21">
-        <v>85</v>
-      </c>
-      <c r="L13" t="s" s="21">
-        <v>86</v>
-      </c>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
       <c r="M13" s="19"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
@@ -2370,7 +2222,7 @@
       <c r="E14" s="21"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="25"/>
+      <c r="H14" s="24"/>
       <c r="I14" s="19"/>
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
@@ -2435,40 +2287,40 @@
       <c r="AH15" s="5"/>
     </row>
     <row r="16" ht="16" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="28"/>
-      <c r="V16" s="28"/>
-      <c r="W16" s="28"/>
-      <c r="X16" s="28"/>
-      <c r="Y16" s="28"/>
-      <c r="Z16" s="28"/>
-      <c r="AA16" s="28"/>
-      <c r="AB16" s="28"/>
-      <c r="AC16" s="28"/>
-      <c r="AD16" s="28"/>
-      <c r="AE16" s="28"/>
-      <c r="AF16" s="28"/>
-      <c r="AG16" s="28"/>
-      <c r="AH16" s="28"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27"/>
+      <c r="AA16" s="27"/>
+      <c r="AB16" s="27"/>
+      <c r="AC16" s="27"/>
+      <c r="AD16" s="27"/>
+      <c r="AE16" s="27"/>
+      <c r="AF16" s="27"/>
+      <c r="AG16" s="27"/>
+      <c r="AH16" s="27"/>
     </row>
     <row r="17" ht="13.8" customHeight="1">
       <c r="A17" s="9"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' into Anim3"
This reverts commit 2ea7e463d9117a3e5d16f07a94b712fa51a25c9e.
</commit_message>
<xml_diff>
--- a/MakeAGame/LubanTool/GameConfig/Datas/Relic.xlsx
+++ b/MakeAGame/LubanTool/GameConfig/Datas/Relic.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
   <si>
     <t>##var</t>
   </si>
@@ -206,72 +206,6 @@
   </si>
   <si>
     <t>Relic6</t>
-  </si>
-  <si>
-    <t>鱼鳞</t>
-  </si>
-  <si>
-    <t>这些鳞片是剥自可怕的巨型海怪。它们可以让你在水中呼吸，并进行长时间的潜水。但取得它们的代价是任何人都无法想象的。</t>
-  </si>
-  <si>
-    <t>每当你造成小于等于{0}点且非Miss伤害时，将伤害提升为{0}</t>
-  </si>
-  <si>
-    <t>Relic7</t>
-  </si>
-  <si>
-    <t>伤害值</t>
-  </si>
-  <si>
-    <t>废品回收机</t>
-  </si>
-  <si>
-    <t>这个破烂回收机可以将无用的垃圾和装置重新变成有用的东西。但使用它需要小心谨慎，因为有时候回收的东西可能远比你想象的更加危险。</t>
-  </si>
-  <si>
-    <t>每使用{0}张死面牌，随机获得一张普通品质的学者牌</t>
-  </si>
-  <si>
-    <t>Relic8</t>
-  </si>
-  <si>
-    <t>使用死面数</t>
-  </si>
-  <si>
-    <t>水晶球</t>
-  </si>
-  <si>
-    <t>这些法珠和水晶球是由神秘巫师制成的。它们能够让你看到未来和未知，但数据可能会来得非常模糊和不可靠。</t>
-  </si>
-  <si>
-    <t>在每场战斗的前{0}秒混沌值损耗减少{1}%</t>
-  </si>
-  <si>
-    <t>Relic9</t>
-  </si>
-  <si>
-    <t>10,10</t>
-  </si>
-  <si>
-    <t>秒数，减少比例</t>
-  </si>
-  <si>
-    <t>符纸</t>
-  </si>
-  <si>
-    <t>些护身符能够保护你不受死气的侵害。当你使用它们时，你会感到一股强烈的保护力量。</t>
-  </si>
-  <si>
-    <t>抵消下{0}次生面牌受到的超过{1}点伤害的攻击</t>
-  </si>
-  <si>
-    <t>Relic10</t>
-  </si>
-  <si>
-    <t>5,10</t>
-  </si>
-  <si>
-    <t>抵消次数，伤害值</t>
   </si>
 </sst>
 </file>
@@ -322,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -443,21 +377,6 @@
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
@@ -471,7 +390,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -544,19 +463,16 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2120,7 +2036,7 @@
       <c r="E9" t="s" s="21">
         <v>62</v>
       </c>
-      <c r="F9" t="s" s="24">
+      <c r="F9" t="s" s="15">
         <v>63</v>
       </c>
       <c r="G9" t="s" s="15">
@@ -2156,33 +2072,17 @@
     </row>
     <row r="10" ht="16" customHeight="1">
       <c r="A10" s="19"/>
-      <c r="B10" s="20">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s" s="21">
-        <v>65</v>
-      </c>
-      <c r="D10" t="s" s="21">
-        <v>66</v>
-      </c>
-      <c r="E10" t="s" s="21">
-        <v>67</v>
-      </c>
-      <c r="F10" t="s" s="24">
-        <v>63</v>
-      </c>
-      <c r="G10" t="s" s="21">
-        <v>68</v>
-      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
-      <c r="K10" t="s" s="21">
-        <v>35</v>
-      </c>
-      <c r="L10" t="s" s="21">
-        <v>69</v>
-      </c>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
       <c r="M10" s="19"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -2208,33 +2108,17 @@
     </row>
     <row r="11" ht="16" customHeight="1">
       <c r="A11" s="19"/>
-      <c r="B11" s="20">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s" s="21">
-        <v>70</v>
-      </c>
-      <c r="D11" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="E11" t="s" s="21">
-        <v>72</v>
-      </c>
-      <c r="F11" t="s" s="24">
-        <v>63</v>
-      </c>
-      <c r="G11" t="s" s="21">
-        <v>73</v>
-      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
-      <c r="K11" t="s" s="21">
-        <v>35</v>
-      </c>
-      <c r="L11" t="s" s="21">
-        <v>74</v>
-      </c>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
       <c r="M11" s="19"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -2260,33 +2144,17 @@
     </row>
     <row r="12" ht="16" customHeight="1">
       <c r="A12" s="19"/>
-      <c r="B12" s="20">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s" s="21">
-        <v>75</v>
-      </c>
-      <c r="D12" t="s" s="21">
-        <v>76</v>
-      </c>
-      <c r="E12" t="s" s="21">
-        <v>77</v>
-      </c>
-      <c r="F12" t="s" s="24">
-        <v>63</v>
-      </c>
-      <c r="G12" t="s" s="21">
-        <v>78</v>
-      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
-      <c r="K12" t="s" s="21">
-        <v>79</v>
-      </c>
-      <c r="L12" t="s" s="21">
-        <v>80</v>
-      </c>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
       <c r="M12" s="19"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
@@ -2312,33 +2180,17 @@
     </row>
     <row r="13" ht="16" customHeight="1">
       <c r="A13" s="19"/>
-      <c r="B13" s="20">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s" s="21">
-        <v>81</v>
-      </c>
-      <c r="D13" t="s" s="21">
-        <v>82</v>
-      </c>
-      <c r="E13" t="s" s="21">
-        <v>83</v>
-      </c>
-      <c r="F13" t="s" s="15">
-        <v>63</v>
-      </c>
-      <c r="G13" t="s" s="21">
-        <v>84</v>
-      </c>
-      <c r="H13" s="25"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="24"/>
       <c r="I13" s="19"/>
       <c r="J13" s="21"/>
-      <c r="K13" t="s" s="21">
-        <v>85</v>
-      </c>
-      <c r="L13" t="s" s="21">
-        <v>86</v>
-      </c>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
       <c r="M13" s="19"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
@@ -2370,7 +2222,7 @@
       <c r="E14" s="21"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="25"/>
+      <c r="H14" s="24"/>
       <c r="I14" s="19"/>
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
@@ -2435,40 +2287,40 @@
       <c r="AH15" s="5"/>
     </row>
     <row r="16" ht="16" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="28"/>
-      <c r="V16" s="28"/>
-      <c r="W16" s="28"/>
-      <c r="X16" s="28"/>
-      <c r="Y16" s="28"/>
-      <c r="Z16" s="28"/>
-      <c r="AA16" s="28"/>
-      <c r="AB16" s="28"/>
-      <c r="AC16" s="28"/>
-      <c r="AD16" s="28"/>
-      <c r="AE16" s="28"/>
-      <c r="AF16" s="28"/>
-      <c r="AG16" s="28"/>
-      <c r="AH16" s="28"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27"/>
+      <c r="AA16" s="27"/>
+      <c r="AB16" s="27"/>
+      <c r="AC16" s="27"/>
+      <c r="AD16" s="27"/>
+      <c r="AE16" s="27"/>
+      <c r="AF16" s="27"/>
+      <c r="AG16" s="27"/>
+      <c r="AH16" s="27"/>
     </row>
     <row r="17" ht="13.8" customHeight="1">
       <c r="A17" s="9"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'main' into Anim3""
This reverts commit 828797f8c123b4caf7dffaf485820f0f39d216e2.
</commit_message>
<xml_diff>
--- a/MakeAGame/LubanTool/GameConfig/Datas/Relic.xlsx
+++ b/MakeAGame/LubanTool/GameConfig/Datas/Relic.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
   <si>
     <t>##var</t>
   </si>
@@ -206,6 +206,72 @@
   </si>
   <si>
     <t>Relic6</t>
+  </si>
+  <si>
+    <t>鱼鳞</t>
+  </si>
+  <si>
+    <t>这些鳞片是剥自可怕的巨型海怪。它们可以让你在水中呼吸，并进行长时间的潜水。但取得它们的代价是任何人都无法想象的。</t>
+  </si>
+  <si>
+    <t>每当你造成小于等于{0}点且非Miss伤害时，将伤害提升为{0}</t>
+  </si>
+  <si>
+    <t>Relic7</t>
+  </si>
+  <si>
+    <t>伤害值</t>
+  </si>
+  <si>
+    <t>废品回收机</t>
+  </si>
+  <si>
+    <t>这个破烂回收机可以将无用的垃圾和装置重新变成有用的东西。但使用它需要小心谨慎，因为有时候回收的东西可能远比你想象的更加危险。</t>
+  </si>
+  <si>
+    <t>每使用{0}张死面牌，随机获得一张普通品质的学者牌</t>
+  </si>
+  <si>
+    <t>Relic8</t>
+  </si>
+  <si>
+    <t>使用死面数</t>
+  </si>
+  <si>
+    <t>水晶球</t>
+  </si>
+  <si>
+    <t>这些法珠和水晶球是由神秘巫师制成的。它们能够让你看到未来和未知，但数据可能会来得非常模糊和不可靠。</t>
+  </si>
+  <si>
+    <t>在每场战斗的前{0}秒混沌值损耗减少{1}%</t>
+  </si>
+  <si>
+    <t>Relic9</t>
+  </si>
+  <si>
+    <t>10,10</t>
+  </si>
+  <si>
+    <t>秒数，减少比例</t>
+  </si>
+  <si>
+    <t>符纸</t>
+  </si>
+  <si>
+    <t>些护身符能够保护你不受死气的侵害。当你使用它们时，你会感到一股强烈的保护力量。</t>
+  </si>
+  <si>
+    <t>抵消下{0}次生面牌受到的超过{1}点伤害的攻击</t>
+  </si>
+  <si>
+    <t>Relic10</t>
+  </si>
+  <si>
+    <t>5,10</t>
+  </si>
+  <si>
+    <t>抵消次数，伤害值</t>
   </si>
 </sst>
 </file>
@@ -256,7 +322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -377,6 +443,21 @@
         <color indexed="11"/>
       </right>
       <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
@@ -390,7 +471,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -463,16 +544,19 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2036,7 +2120,7 @@
       <c r="E9" t="s" s="21">
         <v>62</v>
       </c>
-      <c r="F9" t="s" s="15">
+      <c r="F9" t="s" s="24">
         <v>63</v>
       </c>
       <c r="G9" t="s" s="15">
@@ -2072,17 +2156,33 @@
     </row>
     <row r="10" ht="16" customHeight="1">
       <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
+      <c r="B10" s="20">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s" s="21">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s" s="21">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s" s="21">
+        <v>67</v>
+      </c>
+      <c r="F10" t="s" s="24">
+        <v>63</v>
+      </c>
+      <c r="G10" t="s" s="21">
+        <v>68</v>
+      </c>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
+      <c r="K10" t="s" s="21">
+        <v>35</v>
+      </c>
+      <c r="L10" t="s" s="21">
+        <v>69</v>
+      </c>
       <c r="M10" s="19"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -2108,17 +2208,33 @@
     </row>
     <row r="11" ht="16" customHeight="1">
       <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
+      <c r="B11" s="20">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s" s="21">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="E11" t="s" s="21">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s" s="24">
+        <v>63</v>
+      </c>
+      <c r="G11" t="s" s="21">
+        <v>73</v>
+      </c>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
+      <c r="K11" t="s" s="21">
+        <v>35</v>
+      </c>
+      <c r="L11" t="s" s="21">
+        <v>74</v>
+      </c>
       <c r="M11" s="19"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -2144,17 +2260,33 @@
     </row>
     <row r="12" ht="16" customHeight="1">
       <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
+      <c r="B12" s="20">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s" s="21">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s" s="21">
+        <v>76</v>
+      </c>
+      <c r="E12" t="s" s="21">
+        <v>77</v>
+      </c>
+      <c r="F12" t="s" s="24">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s" s="21">
+        <v>78</v>
+      </c>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
+      <c r="K12" t="s" s="21">
+        <v>79</v>
+      </c>
+      <c r="L12" t="s" s="21">
+        <v>80</v>
+      </c>
       <c r="M12" s="19"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
@@ -2180,17 +2312,33 @@
     </row>
     <row r="13" ht="16" customHeight="1">
       <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="24"/>
+      <c r="B13" s="20">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s" s="21">
+        <v>81</v>
+      </c>
+      <c r="D13" t="s" s="21">
+        <v>82</v>
+      </c>
+      <c r="E13" t="s" s="21">
+        <v>83</v>
+      </c>
+      <c r="F13" t="s" s="15">
+        <v>63</v>
+      </c>
+      <c r="G13" t="s" s="21">
+        <v>84</v>
+      </c>
+      <c r="H13" s="25"/>
       <c r="I13" s="19"/>
       <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
+      <c r="K13" t="s" s="21">
+        <v>85</v>
+      </c>
+      <c r="L13" t="s" s="21">
+        <v>86</v>
+      </c>
       <c r="M13" s="19"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
@@ -2222,7 +2370,7 @@
       <c r="E14" s="21"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="24"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="19"/>
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
@@ -2287,40 +2435,40 @@
       <c r="AH15" s="5"/>
     </row>
     <row r="16" ht="16" customHeight="1">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-      <c r="X16" s="27"/>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="27"/>
-      <c r="AA16" s="27"/>
-      <c r="AB16" s="27"/>
-      <c r="AC16" s="27"/>
-      <c r="AD16" s="27"/>
-      <c r="AE16" s="27"/>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
-      <c r="AH16" s="27"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="28"/>
+      <c r="AB16" s="28"/>
+      <c r="AC16" s="28"/>
+      <c r="AD16" s="28"/>
+      <c r="AE16" s="28"/>
+      <c r="AF16" s="28"/>
+      <c r="AG16" s="28"/>
+      <c r="AH16" s="28"/>
     </row>
     <row r="17" ht="13.8" customHeight="1">
       <c r="A17" s="9"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/544817593/MakeAGame"
This reverts commit c2490bb819a101872d02fe9ee8124e4463ea155f, reversing
changes made to b088bd791962fc3fb5fd2b74a3ef032a56e26737.
</commit_message>
<xml_diff>
--- a/MakeAGame/LubanTool/GameConfig/Datas/Relic.xlsx
+++ b/MakeAGame/LubanTool/GameConfig/Datas/Relic.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
   <si>
     <t>##var</t>
   </si>
@@ -206,6 +206,72 @@
   </si>
   <si>
     <t>Relic6</t>
+  </si>
+  <si>
+    <t>鱼鳞</t>
+  </si>
+  <si>
+    <t>这些鳞片是剥自可怕的巨型海怪。它们可以让你在水中呼吸，并进行长时间的潜水。但取得它们的代价是任何人都无法想象的。</t>
+  </si>
+  <si>
+    <t>每当你造成小于等于{0}点且非Miss伤害时，将伤害提升为{0}</t>
+  </si>
+  <si>
+    <t>Relic7</t>
+  </si>
+  <si>
+    <t>伤害值</t>
+  </si>
+  <si>
+    <t>废品回收机</t>
+  </si>
+  <si>
+    <t>这个破烂回收机可以将无用的垃圾和装置重新变成有用的东西。但使用它需要小心谨慎，因为有时候回收的东西可能远比你想象的更加危险。</t>
+  </si>
+  <si>
+    <t>每使用{0}张死面牌，随机获得一张普通品质的学者牌</t>
+  </si>
+  <si>
+    <t>Relic8</t>
+  </si>
+  <si>
+    <t>使用死面数</t>
+  </si>
+  <si>
+    <t>水晶球</t>
+  </si>
+  <si>
+    <t>这些法珠和水晶球是由神秘巫师制成的。它们能够让你看到未来和未知，但数据可能会来得非常模糊和不可靠。</t>
+  </si>
+  <si>
+    <t>在每场战斗的前{0}秒混沌值损耗减少{1}%</t>
+  </si>
+  <si>
+    <t>Relic9</t>
+  </si>
+  <si>
+    <t>10,10</t>
+  </si>
+  <si>
+    <t>秒数，减少比例</t>
+  </si>
+  <si>
+    <t>符纸</t>
+  </si>
+  <si>
+    <t>些护身符能够保护你不受死气的侵害。当你使用它们时，你会感到一股强烈的保护力量。</t>
+  </si>
+  <si>
+    <t>抵消下{0}次生面牌受到的超过{1}点伤害的攻击</t>
+  </si>
+  <si>
+    <t>Relic10</t>
+  </si>
+  <si>
+    <t>5,10</t>
+  </si>
+  <si>
+    <t>抵消次数，伤害值</t>
   </si>
 </sst>
 </file>
@@ -256,7 +322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -377,6 +443,21 @@
         <color indexed="11"/>
       </right>
       <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
@@ -390,7 +471,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -463,16 +544,19 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2036,7 +2120,7 @@
       <c r="E9" t="s" s="21">
         <v>62</v>
       </c>
-      <c r="F9" t="s" s="15">
+      <c r="F9" t="s" s="24">
         <v>63</v>
       </c>
       <c r="G9" t="s" s="15">
@@ -2072,17 +2156,33 @@
     </row>
     <row r="10" ht="16" customHeight="1">
       <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
+      <c r="B10" s="20">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s" s="21">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s" s="21">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s" s="21">
+        <v>67</v>
+      </c>
+      <c r="F10" t="s" s="24">
+        <v>63</v>
+      </c>
+      <c r="G10" t="s" s="21">
+        <v>68</v>
+      </c>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
+      <c r="K10" t="s" s="21">
+        <v>35</v>
+      </c>
+      <c r="L10" t="s" s="21">
+        <v>69</v>
+      </c>
       <c r="M10" s="19"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -2108,17 +2208,33 @@
     </row>
     <row r="11" ht="16" customHeight="1">
       <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
+      <c r="B11" s="20">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s" s="21">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="E11" t="s" s="21">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s" s="24">
+        <v>63</v>
+      </c>
+      <c r="G11" t="s" s="21">
+        <v>73</v>
+      </c>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
+      <c r="K11" t="s" s="21">
+        <v>35</v>
+      </c>
+      <c r="L11" t="s" s="21">
+        <v>74</v>
+      </c>
       <c r="M11" s="19"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -2144,17 +2260,33 @@
     </row>
     <row r="12" ht="16" customHeight="1">
       <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
+      <c r="B12" s="20">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s" s="21">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s" s="21">
+        <v>76</v>
+      </c>
+      <c r="E12" t="s" s="21">
+        <v>77</v>
+      </c>
+      <c r="F12" t="s" s="24">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s" s="21">
+        <v>78</v>
+      </c>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
+      <c r="K12" t="s" s="21">
+        <v>79</v>
+      </c>
+      <c r="L12" t="s" s="21">
+        <v>80</v>
+      </c>
       <c r="M12" s="19"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
@@ -2180,17 +2312,33 @@
     </row>
     <row r="13" ht="16" customHeight="1">
       <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="24"/>
+      <c r="B13" s="20">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s" s="21">
+        <v>81</v>
+      </c>
+      <c r="D13" t="s" s="21">
+        <v>82</v>
+      </c>
+      <c r="E13" t="s" s="21">
+        <v>83</v>
+      </c>
+      <c r="F13" t="s" s="15">
+        <v>63</v>
+      </c>
+      <c r="G13" t="s" s="21">
+        <v>84</v>
+      </c>
+      <c r="H13" s="25"/>
       <c r="I13" s="19"/>
       <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
+      <c r="K13" t="s" s="21">
+        <v>85</v>
+      </c>
+      <c r="L13" t="s" s="21">
+        <v>86</v>
+      </c>
       <c r="M13" s="19"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
@@ -2222,7 +2370,7 @@
       <c r="E14" s="21"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="24"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="19"/>
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
@@ -2287,40 +2435,40 @@
       <c r="AH15" s="5"/>
     </row>
     <row r="16" ht="16" customHeight="1">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-      <c r="X16" s="27"/>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="27"/>
-      <c r="AA16" s="27"/>
-      <c r="AB16" s="27"/>
-      <c r="AC16" s="27"/>
-      <c r="AD16" s="27"/>
-      <c r="AE16" s="27"/>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
-      <c r="AH16" s="27"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="28"/>
+      <c r="AB16" s="28"/>
+      <c r="AC16" s="28"/>
+      <c r="AD16" s="28"/>
+      <c r="AE16" s="28"/>
+      <c r="AF16" s="28"/>
+      <c r="AG16" s="28"/>
+      <c r="AH16" s="28"/>
     </row>
     <row r="17" ht="13.8" customHeight="1">
       <c r="A17" s="9"/>

</xml_diff>